<commit_message>
Update with final report
</commit_message>
<xml_diff>
--- a/Data/royacafe_data.xlsx
+++ b/Data/royacafe_data.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17426"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JC\Documents\GitHub\OaxacaLeafRust\Data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="19440" windowHeight="8010"/>
+    <workbookView xWindow="600" yWindow="36" windowWidth="19440" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="2" r:id="rId1"/>
@@ -152,9 +157,6 @@
     <t>Tab name:</t>
   </si>
   <si>
-    <t>DM_Garropas</t>
-  </si>
-  <si>
     <t>Fields:</t>
   </si>
   <si>
@@ -234,13 +236,16 @@
   </si>
   <si>
     <t>ROYACAFE indicates that variability index (plant and leaf) values &gt; 10% indicate latent state. Variability index &lt; 10% and severity (leaf and plant) &gt; 30% indicate a moderate-high regional establishment of the disease. Índice de variabilidad es la variación regional relativa a la media. Valores de variabilidad (Hoja y Planta) superiores al 10% indican una condición de foco. Índice de variabilidad menor a 10% y severidad (Hoja y Planta) mayor al 30% indican epidemias establecidas regionalmente de intensidad moderada a alta.</t>
+  </si>
+  <si>
+    <t>royacafe_data</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="19">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -742,57 +747,65 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="43">
-    <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Buena" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Cálculo" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Celda de comprobación" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Celda vinculada" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Encabezado 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Énfasis1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Énfasis2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Énfasis3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Énfasis4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Énfasis5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Énfasis6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Entrada" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Incorrecto" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="42"/>
-    <cellStyle name="Notas" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Salida" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Texto de advertencia" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Texto explicativo" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Título" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Título 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Título 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -834,7 +847,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -866,9 +879,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -900,6 +931,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1075,21 +1124,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.875" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="136.25" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="136.21875" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="16384" width="11" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>27</v>
       </c>
@@ -1097,15 +1146,15 @@
         <v>42661</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75">
+    <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>29</v>
       </c>
@@ -1113,223 +1162,223 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>31</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>32</v>
       </c>
       <c r="B6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>35</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>37</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>38</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>39</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>40</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>41</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>42</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>43</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>44</v>
       </c>
       <c r="B18" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="3" t="s">
+      <c r="B19" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B20" s="4" t="s">
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" s="4" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
-      <c r="A21" t="s">
-        <v>0</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>1</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>2</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>3</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>4</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>5</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>6</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>7</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>8</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>9</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="6"/>
     </row>
   </sheetData>
@@ -1339,27 +1388,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K148"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="10.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="7" width="4.875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="3.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3.88671875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.75" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.77734375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1392,7 +1441,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -1427,7 +1476,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -1462,7 +1511,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1497,7 +1546,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -1532,7 +1581,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -1567,7 +1616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -1602,7 +1651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -1637,7 +1686,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -1672,7 +1721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -1707,7 +1756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -1742,7 +1791,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1777,7 +1826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1812,7 +1861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1847,7 +1896,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -1882,7 +1931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -1917,7 +1966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -1952,7 +2001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -1987,7 +2036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>13</v>
       </c>
@@ -2022,7 +2071,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>10</v>
       </c>
@@ -2057,7 +2106,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>12</v>
       </c>
@@ -2092,7 +2141,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>14</v>
       </c>
@@ -2127,7 +2176,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>13</v>
       </c>
@@ -2162,7 +2211,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>10</v>
       </c>
@@ -2197,7 +2246,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>12</v>
       </c>
@@ -2232,7 +2281,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>14</v>
       </c>
@@ -2267,7 +2316,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>13</v>
       </c>
@@ -2302,7 +2351,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>10</v>
       </c>
@@ -2337,7 +2386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>12</v>
       </c>
@@ -2372,7 +2421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>14</v>
       </c>
@@ -2407,7 +2456,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>13</v>
       </c>
@@ -2442,7 +2491,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="1:11">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>10</v>
       </c>
@@ -2477,7 +2526,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:11">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>12</v>
       </c>
@@ -2512,7 +2561,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="1:11">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>14</v>
       </c>
@@ -2547,7 +2596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:11">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>13</v>
       </c>
@@ -2582,7 +2631,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="36" spans="1:11">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>10</v>
       </c>
@@ -2617,7 +2666,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:11">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>12</v>
       </c>
@@ -2652,7 +2701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:11">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>14</v>
       </c>
@@ -2687,7 +2736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:11">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>13</v>
       </c>
@@ -2722,7 +2771,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="40" spans="1:11">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>10</v>
       </c>
@@ -2757,7 +2806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:11">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>12</v>
       </c>
@@ -2792,7 +2841,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="42" spans="1:11">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>14</v>
       </c>
@@ -2827,7 +2876,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="43" spans="1:11">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>13</v>
       </c>
@@ -2862,7 +2911,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="44" spans="1:11">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>10</v>
       </c>
@@ -2897,7 +2946,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="45" spans="1:11">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>12</v>
       </c>
@@ -2932,7 +2981,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="46" spans="1:11">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>14</v>
       </c>
@@ -2967,7 +3016,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="47" spans="1:11">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>13</v>
       </c>
@@ -3002,7 +3051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:11">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>10</v>
       </c>
@@ -3037,7 +3086,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="49" spans="1:11">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>12</v>
       </c>
@@ -3072,7 +3121,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="50" spans="1:11">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>14</v>
       </c>
@@ -3107,7 +3156,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="51" spans="1:11">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>13</v>
       </c>
@@ -3142,7 +3191,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="52" spans="1:11">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>10</v>
       </c>
@@ -3177,7 +3226,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="53" spans="1:11">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>12</v>
       </c>
@@ -3212,7 +3261,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="54" spans="1:11">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>14</v>
       </c>
@@ -3247,7 +3296,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="55" spans="1:11">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>13</v>
       </c>
@@ -3282,7 +3331,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="56" spans="1:11">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>10</v>
       </c>
@@ -3317,7 +3366,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="57" spans="1:11">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>12</v>
       </c>
@@ -3352,7 +3401,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="58" spans="1:11">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>14</v>
       </c>
@@ -3387,7 +3436,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="59" spans="1:11">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>13</v>
       </c>
@@ -3422,7 +3471,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="60" spans="1:11">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>10</v>
       </c>
@@ -3457,7 +3506,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="61" spans="1:11">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>12</v>
       </c>
@@ -3492,7 +3541,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="62" spans="1:11">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>14</v>
       </c>
@@ -3527,7 +3576,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="63" spans="1:11">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>13</v>
       </c>
@@ -3562,7 +3611,7 @@
         <v>68.3</v>
       </c>
     </row>
-    <row r="64" spans="1:11">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>10</v>
       </c>
@@ -3597,7 +3646,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="65" spans="1:11">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>12</v>
       </c>
@@ -3632,7 +3681,7 @@
         <v>170.5</v>
       </c>
     </row>
-    <row r="66" spans="1:11">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>14</v>
       </c>
@@ -3667,7 +3716,7 @@
         <v>13.5</v>
       </c>
     </row>
-    <row r="67" spans="1:11">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>13</v>
       </c>
@@ -3702,7 +3751,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="68" spans="1:11">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>10</v>
       </c>
@@ -3737,7 +3786,7 @@
         <v>195.5</v>
       </c>
     </row>
-    <row r="69" spans="1:11">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>12</v>
       </c>
@@ -3772,7 +3821,7 @@
         <v>57.5</v>
       </c>
     </row>
-    <row r="70" spans="1:11">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>14</v>
       </c>
@@ -3807,7 +3856,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="71" spans="1:11">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>13</v>
       </c>
@@ -3842,7 +3891,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="72" spans="1:11">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>10</v>
       </c>
@@ -3877,7 +3926,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="73" spans="1:11">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>12</v>
       </c>
@@ -3912,7 +3961,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="74" spans="1:11">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>13</v>
       </c>
@@ -3947,7 +3996,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="75" spans="1:11">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>10</v>
       </c>
@@ -3982,7 +4031,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="76" spans="1:11">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>12</v>
       </c>
@@ -4017,7 +4066,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="77" spans="1:11">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>14</v>
       </c>
@@ -4052,7 +4101,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="78" spans="1:11">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>13</v>
       </c>
@@ -4087,7 +4136,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="79" spans="1:11">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>10</v>
       </c>
@@ -4122,7 +4171,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="80" spans="1:11">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>12</v>
       </c>
@@ -4157,7 +4206,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="81" spans="1:11">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>14</v>
       </c>
@@ -4192,7 +4241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:11">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>13</v>
       </c>
@@ -4227,7 +4276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:11">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>10</v>
       </c>
@@ -4262,7 +4311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:11">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>15</v>
       </c>
@@ -4297,7 +4346,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:11">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>12</v>
       </c>
@@ -4332,7 +4381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:11">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>16</v>
       </c>
@@ -4367,7 +4416,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:11">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>19</v>
       </c>
@@ -4402,7 +4451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:11">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>21</v>
       </c>
@@ -4437,7 +4486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:11">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>18</v>
       </c>
@@ -4472,7 +4521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:11">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>20</v>
       </c>
@@ -4507,7 +4556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:11">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>17</v>
       </c>
@@ -4542,7 +4591,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:11">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>14</v>
       </c>
@@ -4577,7 +4626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:11">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>13</v>
       </c>
@@ -4612,7 +4661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:11">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>10</v>
       </c>
@@ -4647,7 +4696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:11">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>15</v>
       </c>
@@ -4682,7 +4731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:11">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>23</v>
       </c>
@@ -4717,7 +4766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:11">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>12</v>
       </c>
@@ -4752,7 +4801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:11">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>22</v>
       </c>
@@ -4787,7 +4836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:11">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>14</v>
       </c>
@@ -4822,7 +4871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:11">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>13</v>
       </c>
@@ -4857,7 +4906,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:11">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>10</v>
       </c>
@@ -4892,7 +4941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:11">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>23</v>
       </c>
@@ -4927,7 +4976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:11">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>12</v>
       </c>
@@ -4962,7 +5011,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:11">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>22</v>
       </c>
@@ -4997,7 +5046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:11">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>14</v>
       </c>
@@ -5032,7 +5081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:11">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>24</v>
       </c>
@@ -5067,7 +5116,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:11">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>13</v>
       </c>
@@ -5102,7 +5151,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:11">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>26</v>
       </c>
@@ -5137,7 +5186,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="109" spans="1:11">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>10</v>
       </c>
@@ -5172,7 +5221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:11">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>23</v>
       </c>
@@ -5207,7 +5256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:11">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>12</v>
       </c>
@@ -5242,7 +5291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:11">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>25</v>
       </c>
@@ -5277,7 +5326,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="113" spans="1:11">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>22</v>
       </c>
@@ -5312,7 +5361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:11">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>14</v>
       </c>
@@ -5347,7 +5396,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:11">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>24</v>
       </c>
@@ -5382,7 +5431,7 @@
         <v>5.7</v>
       </c>
     </row>
-    <row r="116" spans="1:11">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>13</v>
       </c>
@@ -5417,7 +5466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:11">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>26</v>
       </c>
@@ -5452,7 +5501,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="118" spans="1:11">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>10</v>
       </c>
@@ -5487,7 +5536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:11">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>23</v>
       </c>
@@ -5522,7 +5571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:11">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>12</v>
       </c>
@@ -5557,7 +5606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:11">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>25</v>
       </c>
@@ -5592,7 +5641,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="122" spans="1:11">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>22</v>
       </c>
@@ -5627,7 +5676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:11">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>14</v>
       </c>
@@ -5662,7 +5711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:11">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>24</v>
       </c>
@@ -5697,7 +5746,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="125" spans="1:11">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>13</v>
       </c>
@@ -5732,7 +5781,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:11">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>26</v>
       </c>
@@ -5767,7 +5816,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="127" spans="1:11">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>10</v>
       </c>
@@ -5802,7 +5851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:11">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>23</v>
       </c>
@@ -5837,7 +5886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:11">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>12</v>
       </c>
@@ -5872,7 +5921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:11">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>25</v>
       </c>
@@ -5907,7 +5956,7 @@
         <v>5.2</v>
       </c>
     </row>
-    <row r="131" spans="1:11">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>22</v>
       </c>
@@ -5942,7 +5991,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:11">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>14</v>
       </c>
@@ -5977,7 +6026,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:11">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>24</v>
       </c>
@@ -6012,7 +6061,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:11">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>13</v>
       </c>
@@ -6047,7 +6096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:11">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>26</v>
       </c>
@@ -6082,7 +6131,7 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="136" spans="1:11">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>10</v>
       </c>
@@ -6117,7 +6166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:11">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>23</v>
       </c>
@@ -6152,7 +6201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:11">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>12</v>
       </c>
@@ -6187,7 +6236,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:11">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>25</v>
       </c>
@@ -6222,7 +6271,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="140" spans="1:11">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>22</v>
       </c>
@@ -6257,7 +6306,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:11">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>26</v>
       </c>
@@ -6292,7 +6341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:11">
+    <row r="142" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>25</v>
       </c>
@@ -6327,7 +6376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:11">
+    <row r="143" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>24</v>
       </c>
@@ -6362,7 +6411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:11">
+    <row r="144" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>14</v>
       </c>
@@ -6397,7 +6446,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:11">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>12</v>
       </c>
@@ -6432,9 +6481,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:11">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B146" s="1">
         <v>42597</v>
@@ -6467,7 +6516,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:11">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>13</v>
       </c>
@@ -6502,9 +6551,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:11">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B148" s="1">
         <v>42597</v>

</xml_diff>